<commit_message>
Japan: Reduced corporate rate from 2 to 1
</commit_message>
<xml_diff>
--- a/source_data/Tax Complexity Variable Notes.xlsx
+++ b/source_data/Tax Complexity Variable Notes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\international-tax-competitiveness-index\source_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A085C283-EF06-4914-8B91-5B2DEDEFD941}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BA6A4D4-7B47-4813-97C6-AAA3084278EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" xr2:uid="{799C6252-BD7E-43F6-A84E-AA4474677B14}"/>
   </bookViews>
@@ -152,7 +152,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2551" uniqueCount="402">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2551" uniqueCount="403">
   <si>
     <t>Australia</t>
   </si>
@@ -3413,12 +3413,15 @@
   <si>
     <t>QDMTT + domestic minimum tax</t>
   </si>
+  <si>
+    <t>Two CIT brackets: 23.2% and 19%</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3435,12 +3438,6 @@
     <font>
       <sz val="11"/>
       <name val="Lato"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -3482,7 +3479,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -3501,14 +3498,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
@@ -3893,10 +3882,10 @@
   <dimension ref="A1:L455"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="59" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E414" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E260" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F433" sqref="F433"/>
+      <selection pane="bottomRight" activeCell="F277" sqref="F277"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.899999999999999" x14ac:dyDescent="0.65"/>
@@ -4340,13 +4329,13 @@
       <c r="C12" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="10">
+      <c r="D12">
         <v>2024</v>
       </c>
-      <c r="E12" s="11" t="s">
+      <c r="E12" s="1" t="s">
         <v>384</v>
       </c>
-      <c r="F12" s="10">
+      <c r="F12">
         <v>3</v>
       </c>
       <c r="G12" t="s">
@@ -4786,41 +4775,41 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:12" s="12" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.65">
-      <c r="A24" s="12" t="s">
+    <row r="24" spans="1:12" s="8" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="A24" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="B24" s="12" t="s">
+      <c r="B24" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="C24" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="D24" s="12">
+      <c r="C24" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D24" s="8">
         <v>2024</v>
       </c>
-      <c r="E24" s="13" t="s">
+      <c r="E24" s="7" t="s">
         <v>385</v>
       </c>
-      <c r="F24" s="12">
+      <c r="F24" s="8">
         <v>3</v>
       </c>
-      <c r="G24" s="12" t="s">
-        <v>126</v>
-      </c>
-      <c r="H24" s="12">
-        <v>0</v>
-      </c>
-      <c r="I24" s="12">
-        <v>0</v>
-      </c>
-      <c r="J24" s="12">
-        <v>2</v>
-      </c>
-      <c r="K24" s="12">
-        <v>0</v>
-      </c>
-      <c r="L24" s="12">
+      <c r="G24" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="H24" s="8">
+        <v>0</v>
+      </c>
+      <c r="I24" s="8">
+        <v>0</v>
+      </c>
+      <c r="J24" s="8">
+        <v>2</v>
+      </c>
+      <c r="K24" s="8">
+        <v>0</v>
+      </c>
+      <c r="L24" s="8">
         <v>0</v>
       </c>
     </row>
@@ -5242,41 +5231,41 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:12" s="10" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.65">
-      <c r="A36" s="10" t="s">
+    <row r="36" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="A36" t="s">
         <v>47</v>
       </c>
-      <c r="B36" s="10" t="s">
+      <c r="B36" t="s">
         <v>48</v>
       </c>
-      <c r="C36" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="D36" s="10">
+      <c r="C36" t="s">
+        <v>2</v>
+      </c>
+      <c r="D36">
         <v>2024</v>
       </c>
-      <c r="E36" s="11" t="s">
+      <c r="E36" s="1" t="s">
         <v>386</v>
       </c>
-      <c r="F36" s="10">
-        <v>2</v>
-      </c>
-      <c r="G36" s="10" t="s">
-        <v>126</v>
-      </c>
-      <c r="H36" s="10">
-        <v>0</v>
-      </c>
-      <c r="I36" s="10">
+      <c r="F36">
+        <v>2</v>
+      </c>
+      <c r="G36" t="s">
+        <v>126</v>
+      </c>
+      <c r="H36">
+        <v>0</v>
+      </c>
+      <c r="I36">
         <v>0.03</v>
       </c>
-      <c r="J36" s="10">
-        <v>0</v>
-      </c>
-      <c r="K36" s="10">
-        <v>0</v>
-      </c>
-      <c r="L36" s="10">
+      <c r="J36">
+        <v>0</v>
+      </c>
+      <c r="K36">
+        <v>0</v>
+      </c>
+      <c r="L36">
         <v>2</v>
       </c>
     </row>
@@ -5664,7 +5653,7 @@
       <c r="A47" t="s">
         <v>49</v>
       </c>
-      <c r="B47" s="10" t="s">
+      <c r="B47" t="s">
         <v>50</v>
       </c>
       <c r="C47" t="s">
@@ -5698,41 +5687,41 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:12" s="10" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.65">
-      <c r="A48" s="10" t="s">
+    <row r="48" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="A48" t="s">
         <v>49</v>
       </c>
-      <c r="B48" s="10" t="s">
+      <c r="B48" t="s">
         <v>50</v>
       </c>
-      <c r="C48" s="10" t="s">
+      <c r="C48" t="s">
         <v>3</v>
       </c>
-      <c r="D48" s="10">
+      <c r="D48">
         <v>2024</v>
       </c>
-      <c r="E48" s="11" t="s">
+      <c r="E48" s="1" t="s">
         <v>387</v>
       </c>
-      <c r="F48" s="10">
-        <v>2</v>
-      </c>
-      <c r="G48" s="10" t="s">
-        <v>126</v>
-      </c>
-      <c r="H48" s="10">
-        <v>0</v>
-      </c>
-      <c r="I48" s="10">
+      <c r="F48">
+        <v>2</v>
+      </c>
+      <c r="G48" t="s">
+        <v>126</v>
+      </c>
+      <c r="H48">
+        <v>0</v>
+      </c>
+      <c r="I48">
         <v>1.202</v>
       </c>
-      <c r="J48" s="10">
-        <v>0</v>
-      </c>
-      <c r="K48" s="10">
-        <v>0</v>
-      </c>
-      <c r="L48" s="10">
+      <c r="J48">
+        <v>0</v>
+      </c>
+      <c r="K48">
+        <v>0</v>
+      </c>
+      <c r="L48">
         <v>0</v>
       </c>
     </row>
@@ -6154,41 +6143,41 @@
         <v>2</v>
       </c>
     </row>
-    <row r="60" spans="1:12" s="10" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.65">
-      <c r="A60" s="10" t="s">
+    <row r="60" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="A60" t="s">
         <v>109</v>
       </c>
-      <c r="B60" s="10" t="s">
+      <c r="B60" t="s">
         <v>110</v>
       </c>
-      <c r="C60" s="10" t="s">
+      <c r="C60" t="s">
         <v>33</v>
       </c>
-      <c r="D60" s="10">
+      <c r="D60">
         <v>2024</v>
       </c>
-      <c r="E60" s="10" t="s">
+      <c r="E60" t="s">
         <v>388</v>
       </c>
-      <c r="F60" s="10">
-        <v>1</v>
-      </c>
-      <c r="G60" s="10" t="s">
-        <v>126</v>
-      </c>
-      <c r="H60" s="10">
-        <v>0</v>
-      </c>
-      <c r="I60" s="10">
+      <c r="F60">
+        <v>1</v>
+      </c>
+      <c r="G60" t="s">
+        <v>126</v>
+      </c>
+      <c r="H60">
+        <v>0</v>
+      </c>
+      <c r="I60">
         <v>6.4409999999999998</v>
       </c>
-      <c r="J60" s="10">
-        <v>0</v>
-      </c>
-      <c r="K60" s="10">
-        <v>0</v>
-      </c>
-      <c r="L60" s="10">
+      <c r="J60">
+        <v>0</v>
+      </c>
+      <c r="K60">
+        <v>0</v>
+      </c>
+      <c r="L60">
         <v>2</v>
       </c>
     </row>
@@ -6585,10 +6574,10 @@
       <c r="D71">
         <v>2023</v>
       </c>
-      <c r="E71" s="11" t="s">
+      <c r="E71" s="1" t="s">
         <v>378</v>
       </c>
-      <c r="F71" s="10">
+      <c r="F71">
         <v>0</v>
       </c>
       <c r="G71" t="s">
@@ -7041,10 +7030,10 @@
       <c r="D83">
         <v>2023</v>
       </c>
-      <c r="E83" s="11" t="s">
+      <c r="E83" s="1" t="s">
         <v>389</v>
       </c>
-      <c r="F83" s="10">
+      <c r="F83">
         <v>3</v>
       </c>
       <c r="G83" t="s">
@@ -7079,10 +7068,10 @@
       <c r="D84">
         <v>2024</v>
       </c>
-      <c r="E84" s="11" t="s">
+      <c r="E84" s="1" t="s">
         <v>389</v>
       </c>
-      <c r="F84" s="10">
+      <c r="F84">
         <v>3</v>
       </c>
       <c r="G84" t="s">
@@ -7957,41 +7946,41 @@
         <v>2</v>
       </c>
     </row>
-    <row r="108" spans="1:12" s="10" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.65">
-      <c r="A108" s="10" t="s">
+    <row r="108" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="A108" t="s">
         <v>55</v>
       </c>
-      <c r="B108" s="10" t="s">
+      <c r="B108" t="s">
         <v>56</v>
       </c>
-      <c r="C108" s="10" t="s">
+      <c r="C108" t="s">
         <v>6</v>
       </c>
-      <c r="D108" s="10">
+      <c r="D108">
         <v>2024</v>
       </c>
-      <c r="E108" s="10" t="s">
+      <c r="E108" t="s">
         <v>388</v>
       </c>
-      <c r="F108" s="10">
-        <v>1</v>
-      </c>
-      <c r="G108" s="10" t="s">
-        <v>126</v>
-      </c>
-      <c r="H108" s="10">
-        <v>0</v>
-      </c>
-      <c r="I108" s="10">
-        <v>0</v>
-      </c>
-      <c r="J108" s="10">
-        <v>0</v>
-      </c>
-      <c r="K108" s="10">
-        <v>0</v>
-      </c>
-      <c r="L108" s="10">
+      <c r="F108">
+        <v>1</v>
+      </c>
+      <c r="G108" t="s">
+        <v>126</v>
+      </c>
+      <c r="H108">
+        <v>0</v>
+      </c>
+      <c r="I108">
+        <v>0</v>
+      </c>
+      <c r="J108">
+        <v>0</v>
+      </c>
+      <c r="K108">
+        <v>0</v>
+      </c>
+      <c r="L108">
         <v>2</v>
       </c>
     </row>
@@ -8413,41 +8402,41 @@
         <v>1</v>
       </c>
     </row>
-    <row r="120" spans="1:12" s="10" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.65">
-      <c r="A120" s="10" t="s">
+    <row r="120" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="A120" t="s">
         <v>65</v>
       </c>
-      <c r="B120" s="10" t="s">
+      <c r="B120" t="s">
         <v>66</v>
       </c>
-      <c r="C120" s="10" t="s">
+      <c r="C120" t="s">
         <v>11</v>
       </c>
-      <c r="D120" s="10">
+      <c r="D120">
         <v>2024</v>
       </c>
-      <c r="E120" s="10" t="s">
+      <c r="E120" t="s">
         <v>388</v>
       </c>
-      <c r="F120" s="10">
-        <v>1</v>
-      </c>
-      <c r="G120" s="11" t="s">
+      <c r="F120">
+        <v>1</v>
+      </c>
+      <c r="G120" s="1" t="s">
         <v>375</v>
       </c>
-      <c r="H120" s="10">
+      <c r="H120">
         <v>5.5</v>
       </c>
-      <c r="I120" s="10">
-        <v>0</v>
-      </c>
-      <c r="J120" s="10">
+      <c r="I120">
+        <v>0</v>
+      </c>
+      <c r="J120">
         <v>5.5</v>
       </c>
-      <c r="K120" s="10">
-        <v>0</v>
-      </c>
-      <c r="L120" s="10">
+      <c r="K120">
+        <v>0</v>
+      </c>
+      <c r="L120">
         <v>1</v>
       </c>
     </row>
@@ -8869,41 +8858,41 @@
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="1:12" s="10" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.65">
-      <c r="A132" s="10" t="s">
+    <row r="132" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="A132" t="s">
         <v>57</v>
       </c>
-      <c r="B132" s="10" t="s">
+      <c r="B132" t="s">
         <v>58</v>
       </c>
-      <c r="C132" s="10" t="s">
+      <c r="C132" t="s">
         <v>7</v>
       </c>
-      <c r="D132" s="10">
+      <c r="D132">
         <v>2024</v>
       </c>
-      <c r="E132" s="10" t="s">
+      <c r="E132" t="s">
         <v>388</v>
       </c>
-      <c r="F132" s="10">
-        <v>1</v>
-      </c>
-      <c r="G132" s="10" t="s">
-        <v>126</v>
-      </c>
-      <c r="H132" s="10">
-        <v>0</v>
-      </c>
-      <c r="I132" s="10">
+      <c r="F132">
+        <v>1</v>
+      </c>
+      <c r="G132" t="s">
+        <v>126</v>
+      </c>
+      <c r="H132">
+        <v>0</v>
+      </c>
+      <c r="I132">
         <v>5.4029999999999996</v>
       </c>
-      <c r="J132" s="10">
+      <c r="J132">
         <v>6.23</v>
       </c>
-      <c r="K132" s="10">
-        <v>0</v>
-      </c>
-      <c r="L132" s="10">
+      <c r="K132">
+        <v>0</v>
+      </c>
+      <c r="L132">
         <v>0</v>
       </c>
     </row>
@@ -9642,10 +9631,10 @@
       <c r="D152">
         <v>2021</v>
       </c>
-      <c r="E152" s="13" t="s">
+      <c r="E152" s="7" t="s">
         <v>338</v>
       </c>
-      <c r="F152" s="10">
+      <c r="F152">
         <v>1</v>
       </c>
       <c r="G152" t="s">
@@ -10187,41 +10176,41 @@
         <v>2</v>
       </c>
     </row>
-    <row r="167" spans="1:12" s="10" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.65">
-      <c r="A167" s="10" t="s">
+    <row r="167" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="A167" t="s">
         <v>61</v>
       </c>
-      <c r="B167" s="10" t="s">
+      <c r="B167" t="s">
         <v>62</v>
       </c>
-      <c r="C167" s="10" t="s">
+      <c r="C167" t="s">
         <v>9</v>
       </c>
-      <c r="D167" s="10">
+      <c r="D167">
         <v>2024</v>
       </c>
-      <c r="E167" s="10" t="s">
+      <c r="E167" t="s">
         <v>388</v>
       </c>
-      <c r="F167" s="10">
-        <v>1</v>
-      </c>
-      <c r="G167" s="10" t="s">
-        <v>126</v>
-      </c>
-      <c r="H167" s="10">
-        <v>0</v>
-      </c>
-      <c r="I167" s="10">
-        <v>0</v>
-      </c>
-      <c r="J167" s="10">
-        <v>0</v>
-      </c>
-      <c r="K167" s="10">
-        <v>0</v>
-      </c>
-      <c r="L167" s="10">
+      <c r="F167">
+        <v>1</v>
+      </c>
+      <c r="G167" t="s">
+        <v>126</v>
+      </c>
+      <c r="H167">
+        <v>0</v>
+      </c>
+      <c r="I167">
+        <v>0</v>
+      </c>
+      <c r="J167">
+        <v>0</v>
+      </c>
+      <c r="K167">
+        <v>0</v>
+      </c>
+      <c r="L167">
         <v>2</v>
       </c>
     </row>
@@ -10643,79 +10632,79 @@
         <v>3</v>
       </c>
     </row>
-    <row r="179" spans="1:12" s="10" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.65">
-      <c r="A179" s="10" t="s">
+    <row r="179" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="A179" t="s">
         <v>63</v>
       </c>
-      <c r="B179" s="10" t="s">
+      <c r="B179" t="s">
         <v>64</v>
       </c>
-      <c r="C179" s="10" t="s">
+      <c r="C179" t="s">
         <v>10</v>
       </c>
-      <c r="D179" s="10">
+      <c r="D179">
         <v>2024</v>
       </c>
-      <c r="E179" s="10" t="s">
+      <c r="E179" t="s">
         <v>390</v>
       </c>
-      <c r="F179" s="10">
-        <v>2</v>
-      </c>
-      <c r="G179" s="11" t="s">
+      <c r="F179">
+        <v>2</v>
+      </c>
+      <c r="G179" s="1" t="s">
         <v>372</v>
       </c>
-      <c r="H179" s="10">
+      <c r="H179">
         <v>3.3</v>
       </c>
-      <c r="I179" s="10">
+      <c r="I179">
         <v>0.95699999999999996</v>
       </c>
-      <c r="J179" s="10">
-        <v>0</v>
-      </c>
-      <c r="K179" s="10">
-        <v>0</v>
-      </c>
-      <c r="L179" s="10">
+      <c r="J179">
+        <v>0</v>
+      </c>
+      <c r="K179">
+        <v>0</v>
+      </c>
+      <c r="L179">
         <v>3</v>
       </c>
     </row>
-    <row r="180" spans="1:12" s="14" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.65">
-      <c r="A180" s="14" t="s">
+    <row r="180" spans="1:12" s="10" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="A180" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="B180" s="14" t="s">
+      <c r="B180" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="C180" s="14" t="s">
+      <c r="C180" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="D180" s="14">
+      <c r="D180" s="10">
         <v>2024</v>
       </c>
-      <c r="E180" s="14" t="s">
+      <c r="E180" s="10" t="s">
         <v>397</v>
       </c>
-      <c r="F180" s="14">
+      <c r="F180" s="10">
         <v>4</v>
       </c>
-      <c r="G180" s="15" t="s">
+      <c r="G180" s="11" t="s">
         <v>398</v>
       </c>
-      <c r="H180" s="14">
+      <c r="H180" s="10">
         <v>3.3</v>
       </c>
-      <c r="I180" s="14">
+      <c r="I180" s="10">
         <v>0.95699999999999996</v>
       </c>
-      <c r="J180" s="14">
-        <v>0</v>
-      </c>
-      <c r="K180" s="14">
-        <v>0</v>
-      </c>
-      <c r="L180" s="14">
+      <c r="J180" s="10">
+        <v>0</v>
+      </c>
+      <c r="K180" s="10">
+        <v>0</v>
+      </c>
+      <c r="L180" s="10">
         <v>3</v>
       </c>
     </row>
@@ -11093,38 +11082,38 @@
         <v>1</v>
       </c>
     </row>
-    <row r="191" spans="1:12" s="10" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.65">
-      <c r="A191" s="10" t="s">
+    <row r="191" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="A191" t="s">
         <v>113</v>
       </c>
-      <c r="B191" s="10" t="s">
+      <c r="B191" t="s">
         <v>114</v>
       </c>
-      <c r="C191" s="10" t="s">
+      <c r="C191" t="s">
         <v>35</v>
       </c>
-      <c r="D191" s="10">
+      <c r="D191">
         <v>2024</v>
       </c>
-      <c r="E191" s="11" t="s">
+      <c r="E191" s="1" t="s">
         <v>391</v>
       </c>
-      <c r="F191" s="10">
+      <c r="F191">
         <v>3</v>
       </c>
-      <c r="G191" s="10" t="s">
-        <v>126</v>
-      </c>
-      <c r="H191" s="10">
-        <v>0</v>
-      </c>
-      <c r="I191" s="10">
-        <v>0</v>
-      </c>
-      <c r="K191" s="10">
-        <v>0</v>
-      </c>
-      <c r="L191" s="10">
+      <c r="G191" t="s">
+        <v>126</v>
+      </c>
+      <c r="H191">
+        <v>0</v>
+      </c>
+      <c r="I191">
+        <v>0</v>
+      </c>
+      <c r="K191">
+        <v>0</v>
+      </c>
+      <c r="L191">
         <v>1</v>
       </c>
     </row>
@@ -11537,38 +11526,38 @@
         <v>2</v>
       </c>
     </row>
-    <row r="203" spans="1:12" s="10" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.65">
-      <c r="A203" s="10" t="s">
+    <row r="203" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="A203" t="s">
         <v>67</v>
       </c>
-      <c r="B203" s="10" t="s">
+      <c r="B203" t="s">
         <v>68</v>
       </c>
-      <c r="C203" s="10" t="s">
+      <c r="C203" t="s">
         <v>12</v>
       </c>
-      <c r="D203" s="10">
+      <c r="D203">
         <v>2024</v>
       </c>
-      <c r="E203" s="10" t="s">
+      <c r="E203" t="s">
         <v>388</v>
       </c>
-      <c r="F203" s="10">
-        <v>1</v>
-      </c>
-      <c r="G203" s="10" t="s">
-        <v>126</v>
-      </c>
-      <c r="H203" s="10">
-        <v>0</v>
-      </c>
-      <c r="I203" s="10">
+      <c r="F203">
+        <v>1</v>
+      </c>
+      <c r="G203" t="s">
+        <v>126</v>
+      </c>
+      <c r="H203">
+        <v>0</v>
+      </c>
+      <c r="I203">
         <v>1.0349999999999999</v>
       </c>
-      <c r="K203" s="10">
-        <v>0</v>
-      </c>
-      <c r="L203" s="10">
+      <c r="K203">
+        <v>0</v>
+      </c>
+      <c r="L203">
         <v>2</v>
       </c>
     </row>
@@ -11987,41 +11976,41 @@
         <v>2</v>
       </c>
     </row>
-    <row r="215" spans="1:12" s="10" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.65">
-      <c r="A215" s="10" t="s">
+    <row r="215" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="A215" t="s">
         <v>69</v>
       </c>
-      <c r="B215" s="10" t="s">
+      <c r="B215" t="s">
         <v>70</v>
       </c>
-      <c r="C215" s="10" t="s">
+      <c r="C215" t="s">
         <v>13</v>
       </c>
-      <c r="D215" s="10">
+      <c r="D215">
         <v>2024</v>
       </c>
-      <c r="E215" s="10" t="s">
+      <c r="E215" t="s">
         <v>392</v>
       </c>
-      <c r="F215" s="10">
-        <v>1</v>
-      </c>
-      <c r="G215" s="10" t="s">
-        <v>126</v>
-      </c>
-      <c r="H215" s="10">
-        <v>0</v>
-      </c>
-      <c r="I215" s="10">
+      <c r="F215">
+        <v>1</v>
+      </c>
+      <c r="G215" t="s">
+        <v>126</v>
+      </c>
+      <c r="H215">
+        <v>0</v>
+      </c>
+      <c r="I215">
         <v>0.14000000000000001</v>
       </c>
-      <c r="J215" s="10">
-        <v>0</v>
-      </c>
-      <c r="K215" s="10">
+      <c r="J215">
+        <v>0</v>
+      </c>
+      <c r="K215">
         <v>0.16800000000000001</v>
       </c>
-      <c r="L215" s="10">
+      <c r="L215">
         <v>2</v>
       </c>
     </row>
@@ -12443,41 +12432,41 @@
         <v>2</v>
       </c>
     </row>
-    <row r="227" spans="1:12" s="10" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.65">
-      <c r="A227" s="10" t="s">
+    <row r="227" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="A227" t="s">
         <v>73</v>
       </c>
-      <c r="B227" s="10" t="s">
+      <c r="B227" t="s">
         <v>74</v>
       </c>
-      <c r="C227" s="10" t="s">
+      <c r="C227" t="s">
         <v>15</v>
       </c>
-      <c r="D227" s="10">
+      <c r="D227">
         <v>2024</v>
       </c>
-      <c r="E227" s="10" t="s">
+      <c r="E227" t="s">
         <v>393</v>
       </c>
-      <c r="F227" s="10">
-        <v>2</v>
-      </c>
-      <c r="G227" s="10" t="s">
-        <v>126</v>
-      </c>
-      <c r="H227" s="10">
-        <v>0</v>
-      </c>
-      <c r="I227" s="10">
-        <v>0</v>
-      </c>
-      <c r="J227" s="10">
-        <v>0</v>
-      </c>
-      <c r="K227" s="10">
-        <v>0</v>
-      </c>
-      <c r="L227" s="10">
+      <c r="F227">
+        <v>2</v>
+      </c>
+      <c r="G227" t="s">
+        <v>126</v>
+      </c>
+      <c r="H227">
+        <v>0</v>
+      </c>
+      <c r="I227">
+        <v>0</v>
+      </c>
+      <c r="J227">
+        <v>0</v>
+      </c>
+      <c r="K227">
+        <v>0</v>
+      </c>
+      <c r="L227">
         <v>2</v>
       </c>
     </row>
@@ -13805,41 +13794,41 @@
         <v>3</v>
       </c>
     </row>
-    <row r="263" spans="1:12" s="10" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.65">
-      <c r="A263" s="10" t="s">
+    <row r="263" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="A263" t="s">
         <v>77</v>
       </c>
-      <c r="B263" s="10" t="s">
+      <c r="B263" t="s">
         <v>78</v>
       </c>
-      <c r="C263" s="10" t="s">
+      <c r="C263" t="s">
         <v>17</v>
       </c>
-      <c r="D263" s="10">
+      <c r="D263">
         <v>2024</v>
       </c>
-      <c r="E263" s="10" t="s">
+      <c r="E263" t="s">
         <v>394</v>
       </c>
-      <c r="F263" s="10">
-        <v>2</v>
-      </c>
-      <c r="G263" s="10" t="s">
-        <v>126</v>
-      </c>
-      <c r="H263" s="10">
-        <v>0</v>
-      </c>
-      <c r="I263" s="10">
+      <c r="F263">
+        <v>2</v>
+      </c>
+      <c r="G263" t="s">
+        <v>126</v>
+      </c>
+      <c r="H263">
+        <v>0</v>
+      </c>
+      <c r="I263">
         <v>4.468</v>
       </c>
-      <c r="J263" s="10">
-        <v>0</v>
-      </c>
-      <c r="K263" s="10">
-        <v>0</v>
-      </c>
-      <c r="L263" s="10">
+      <c r="J263">
+        <v>0</v>
+      </c>
+      <c r="K263">
+        <v>0</v>
+      </c>
+      <c r="L263">
         <v>3</v>
       </c>
     </row>
@@ -14261,41 +14250,41 @@
         <v>1</v>
       </c>
     </row>
-    <row r="275" spans="1:12" s="10" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.65">
-      <c r="A275" s="10" t="s">
+    <row r="275" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="A275" t="s">
         <v>79</v>
       </c>
-      <c r="B275" s="10" t="s">
+      <c r="B275" t="s">
         <v>80</v>
       </c>
-      <c r="C275" s="10" t="s">
+      <c r="C275" t="s">
         <v>18</v>
       </c>
-      <c r="D275" s="10">
+      <c r="D275">
         <v>2024</v>
       </c>
-      <c r="E275" s="10" t="s">
+      <c r="E275" t="s">
         <v>380</v>
       </c>
-      <c r="F275" s="10">
-        <v>2</v>
-      </c>
-      <c r="G275" s="10" t="s">
-        <v>126</v>
-      </c>
-      <c r="H275" s="10">
-        <v>0</v>
-      </c>
-      <c r="I275" s="10">
+      <c r="F275">
+        <v>2</v>
+      </c>
+      <c r="G275" t="s">
+        <v>126</v>
+      </c>
+      <c r="H275">
+        <v>0</v>
+      </c>
+      <c r="I275">
         <v>0.217</v>
       </c>
-      <c r="J275" s="10">
+      <c r="J275">
         <v>2.1</v>
       </c>
-      <c r="K275" s="10">
-        <v>0</v>
-      </c>
-      <c r="L275" s="10">
+      <c r="K275">
+        <v>0</v>
+      </c>
+      <c r="L275">
         <v>1</v>
       </c>
     </row>
@@ -14313,10 +14302,10 @@
         <v>2025</v>
       </c>
       <c r="E276" s="3" t="s">
-        <v>380</v>
+        <v>402</v>
       </c>
       <c r="F276" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G276" s="3" t="s">
         <v>126</v>
@@ -15591,41 +15580,41 @@
         <v>3</v>
       </c>
     </row>
-    <row r="310" spans="1:12" s="10" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.65">
-      <c r="A310" s="10" t="s">
+    <row r="310" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="A310" t="s">
         <v>87</v>
       </c>
-      <c r="B310" s="10" t="s">
+      <c r="B310" t="s">
         <v>88</v>
       </c>
-      <c r="C310" s="10" t="s">
+      <c r="C310" t="s">
         <v>22</v>
       </c>
-      <c r="D310" s="10">
+      <c r="D310">
         <v>2024</v>
       </c>
-      <c r="E310" s="10" t="s">
+      <c r="E310" t="s">
         <v>388</v>
       </c>
-      <c r="F310" s="10">
-        <v>2</v>
-      </c>
-      <c r="G310" s="10" t="s">
+      <c r="F310">
+        <v>2</v>
+      </c>
+      <c r="G310" t="s">
         <v>373</v>
       </c>
-      <c r="H310" s="10">
+      <c r="H310">
         <v>7</v>
       </c>
-      <c r="I310" s="10">
+      <c r="I310">
         <v>0.104</v>
       </c>
-      <c r="J310" s="10">
-        <v>0</v>
-      </c>
-      <c r="K310" s="10">
-        <v>0</v>
-      </c>
-      <c r="L310" s="10">
+      <c r="J310">
+        <v>0</v>
+      </c>
+      <c r="K310">
+        <v>0</v>
+      </c>
+      <c r="L310">
         <v>3</v>
       </c>
     </row>
@@ -16956,41 +16945,41 @@
         <v>1</v>
       </c>
     </row>
-    <row r="346" spans="1:12" s="10" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.65">
-      <c r="A346" s="10" t="s">
+    <row r="346" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="A346" t="s">
         <v>91</v>
       </c>
-      <c r="B346" s="10" t="s">
+      <c r="B346" t="s">
         <v>92</v>
       </c>
-      <c r="C346" s="10" t="s">
+      <c r="C346" t="s">
         <v>24</v>
       </c>
-      <c r="D346" s="10">
+      <c r="D346">
         <v>2024</v>
       </c>
-      <c r="E346" s="10" t="s">
+      <c r="E346" t="s">
         <v>388</v>
       </c>
-      <c r="F346" s="10">
-        <v>2</v>
-      </c>
-      <c r="G346" s="10" t="s">
-        <v>126</v>
-      </c>
-      <c r="H346" s="10">
-        <v>0</v>
-      </c>
-      <c r="I346" s="10">
-        <v>0</v>
-      </c>
-      <c r="J346" s="10">
-        <v>0</v>
-      </c>
-      <c r="K346" s="10">
-        <v>0</v>
-      </c>
-      <c r="L346" s="10">
+      <c r="F346">
+        <v>2</v>
+      </c>
+      <c r="G346" t="s">
+        <v>126</v>
+      </c>
+      <c r="H346">
+        <v>0</v>
+      </c>
+      <c r="I346">
+        <v>0</v>
+      </c>
+      <c r="J346">
+        <v>0</v>
+      </c>
+      <c r="K346">
+        <v>0</v>
+      </c>
+      <c r="L346">
         <v>1</v>
       </c>
     </row>
@@ -17412,41 +17401,41 @@
         <v>2</v>
       </c>
     </row>
-    <row r="358" spans="1:12" s="10" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.65">
-      <c r="A358" s="10" t="s">
+    <row r="358" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="A358" t="s">
         <v>95</v>
       </c>
-      <c r="B358" s="10" t="s">
+      <c r="B358" t="s">
         <v>96</v>
       </c>
-      <c r="C358" s="10" t="s">
+      <c r="C358" t="s">
         <v>26</v>
       </c>
-      <c r="D358" s="10">
+      <c r="D358">
         <v>2024</v>
       </c>
-      <c r="E358" s="10" t="s">
+      <c r="E358" t="s">
         <v>388</v>
       </c>
-      <c r="F358" s="10">
-        <v>1</v>
-      </c>
-      <c r="G358" s="10" t="s">
-        <v>126</v>
-      </c>
-      <c r="H358" s="10">
-        <v>0</v>
-      </c>
-      <c r="I358" s="10">
-        <v>0</v>
-      </c>
-      <c r="J358" s="10">
-        <v>0</v>
-      </c>
-      <c r="K358" s="10">
-        <v>0</v>
-      </c>
-      <c r="L358" s="10">
+      <c r="F358">
+        <v>1</v>
+      </c>
+      <c r="G358" t="s">
+        <v>126</v>
+      </c>
+      <c r="H358">
+        <v>0</v>
+      </c>
+      <c r="I358">
+        <v>0</v>
+      </c>
+      <c r="J358">
+        <v>0</v>
+      </c>
+      <c r="K358">
+        <v>0</v>
+      </c>
+      <c r="L358">
         <v>2</v>
       </c>
     </row>
@@ -18324,41 +18313,41 @@
         <v>2</v>
       </c>
     </row>
-    <row r="382" spans="1:12" s="10" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.65">
-      <c r="A382" s="10" t="s">
+    <row r="382" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="A382" t="s">
         <v>97</v>
       </c>
-      <c r="B382" s="10" t="s">
+      <c r="B382" t="s">
         <v>98</v>
       </c>
-      <c r="C382" s="10" t="s">
+      <c r="C382" t="s">
         <v>27</v>
       </c>
-      <c r="D382" s="10">
+      <c r="D382">
         <v>2024</v>
       </c>
-      <c r="E382" s="12" t="s">
+      <c r="E382" s="8" t="s">
         <v>383</v>
       </c>
-      <c r="F382" s="12">
-        <v>2</v>
-      </c>
-      <c r="G382" s="10" t="s">
-        <v>126</v>
-      </c>
-      <c r="H382" s="10">
-        <v>0</v>
-      </c>
-      <c r="I382" s="10">
-        <v>0</v>
-      </c>
-      <c r="J382" s="10">
-        <v>0</v>
-      </c>
-      <c r="K382" s="10">
-        <v>0</v>
-      </c>
-      <c r="L382" s="10">
+      <c r="F382" s="8">
+        <v>2</v>
+      </c>
+      <c r="G382" t="s">
+        <v>126</v>
+      </c>
+      <c r="H382">
+        <v>0</v>
+      </c>
+      <c r="I382">
+        <v>0</v>
+      </c>
+      <c r="J382">
+        <v>0</v>
+      </c>
+      <c r="K382">
+        <v>0</v>
+      </c>
+      <c r="L382">
         <v>2</v>
       </c>
     </row>
@@ -18780,41 +18769,41 @@
         <v>2</v>
       </c>
     </row>
-    <row r="394" spans="1:12" s="10" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.65">
-      <c r="A394" s="10" t="s">
+    <row r="394" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="A394" t="s">
         <v>99</v>
       </c>
-      <c r="B394" s="10" t="s">
+      <c r="B394" t="s">
         <v>100</v>
       </c>
-      <c r="C394" s="10" t="s">
+      <c r="C394" t="s">
         <v>28</v>
       </c>
-      <c r="D394" s="10">
+      <c r="D394">
         <v>2024</v>
       </c>
-      <c r="E394" s="10" t="s">
+      <c r="E394" t="s">
         <v>388</v>
       </c>
-      <c r="F394" s="10">
+      <c r="F394">
         <v>6</v>
       </c>
-      <c r="G394" s="11" t="s">
+      <c r="G394" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="H394" s="10">
+      <c r="H394">
         <v>9</v>
       </c>
-      <c r="I394" s="10">
+      <c r="I394">
         <v>0.55600000000000005</v>
       </c>
-      <c r="J394" s="10">
-        <v>0</v>
-      </c>
-      <c r="K394" s="10">
-        <v>0</v>
-      </c>
-      <c r="L394" s="10">
+      <c r="J394">
+        <v>0</v>
+      </c>
+      <c r="K394">
+        <v>0</v>
+      </c>
+      <c r="L394">
         <v>2</v>
       </c>
     </row>
@@ -19236,41 +19225,41 @@
         <v>2</v>
       </c>
     </row>
-    <row r="406" spans="1:12" s="10" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.65">
-      <c r="A406" s="10" t="s">
+    <row r="406" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="A406" t="s">
         <v>107</v>
       </c>
-      <c r="B406" s="10" t="s">
+      <c r="B406" t="s">
         <v>108</v>
       </c>
-      <c r="C406" s="10" t="s">
+      <c r="C406" t="s">
         <v>32</v>
       </c>
-      <c r="D406" s="10">
+      <c r="D406">
         <v>2024</v>
       </c>
-      <c r="E406" s="10" t="s">
+      <c r="E406" t="s">
         <v>388</v>
       </c>
-      <c r="F406" s="10">
-        <v>1</v>
-      </c>
-      <c r="G406" s="10" t="s">
-        <v>126</v>
-      </c>
-      <c r="H406" s="10">
-        <v>0</v>
-      </c>
-      <c r="I406" s="10">
-        <v>0</v>
-      </c>
-      <c r="J406" s="10">
-        <v>0</v>
-      </c>
-      <c r="K406" s="10">
+      <c r="F406">
+        <v>1</v>
+      </c>
+      <c r="G406" t="s">
+        <v>126</v>
+      </c>
+      <c r="H406">
+        <v>0</v>
+      </c>
+      <c r="I406">
+        <v>0</v>
+      </c>
+      <c r="J406">
+        <v>0</v>
+      </c>
+      <c r="K406">
         <v>-3.3000000000000002E-2</v>
       </c>
-      <c r="L406" s="10">
+      <c r="L406">
         <v>2</v>
       </c>
     </row>
@@ -19692,41 +19681,41 @@
         <v>2</v>
       </c>
     </row>
-    <row r="418" spans="1:12" s="10" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.65">
-      <c r="A418" s="10" t="s">
+    <row r="418" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="A418" t="s">
         <v>103</v>
       </c>
-      <c r="B418" s="10" t="s">
+      <c r="B418" t="s">
         <v>104</v>
       </c>
-      <c r="C418" s="10" t="s">
+      <c r="C418" t="s">
         <v>30</v>
       </c>
-      <c r="D418" s="10">
+      <c r="D418">
         <v>2024</v>
       </c>
-      <c r="E418" s="10" t="s">
+      <c r="E418" t="s">
         <v>388</v>
       </c>
-      <c r="F418" s="10">
-        <v>1</v>
-      </c>
-      <c r="G418" s="10" t="s">
-        <v>126</v>
-      </c>
-      <c r="H418" s="10">
-        <v>0</v>
-      </c>
-      <c r="I418" s="10">
+      <c r="F418">
+        <v>1</v>
+      </c>
+      <c r="G418" t="s">
+        <v>126</v>
+      </c>
+      <c r="H418">
+        <v>0</v>
+      </c>
+      <c r="I418">
         <v>1.4E-2</v>
       </c>
-      <c r="J418" s="10">
-        <v>0</v>
-      </c>
-      <c r="K418" s="10">
-        <v>0</v>
-      </c>
-      <c r="L418" s="10">
+      <c r="J418">
+        <v>0</v>
+      </c>
+      <c r="K418">
+        <v>0</v>
+      </c>
+      <c r="L418">
         <v>2</v>
       </c>
     </row>
@@ -20148,41 +20137,41 @@
         <v>2</v>
       </c>
     </row>
-    <row r="430" spans="1:12" s="10" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.65">
-      <c r="A430" s="10" t="s">
+    <row r="430" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="A430" t="s">
         <v>101</v>
       </c>
-      <c r="B430" s="10" t="s">
+      <c r="B430" t="s">
         <v>102</v>
       </c>
-      <c r="C430" s="10" t="s">
+      <c r="C430" t="s">
         <v>29</v>
       </c>
-      <c r="D430" s="10">
+      <c r="D430">
         <v>2024</v>
       </c>
-      <c r="E430" s="10" t="s">
+      <c r="E430" t="s">
         <v>395</v>
       </c>
-      <c r="F430" s="10">
-        <v>2</v>
-      </c>
-      <c r="G430" s="10" t="s">
-        <v>126</v>
-      </c>
-      <c r="H430" s="10">
-        <v>0</v>
-      </c>
-      <c r="I430" s="10">
+      <c r="F430">
+        <v>2</v>
+      </c>
+      <c r="G430" t="s">
+        <v>126</v>
+      </c>
+      <c r="H430">
+        <v>0</v>
+      </c>
+      <c r="I430">
         <v>0.83399999999999996</v>
       </c>
-      <c r="J430" s="10">
-        <v>0</v>
-      </c>
-      <c r="K430" s="10">
-        <v>0</v>
-      </c>
-      <c r="L430" s="10">
+      <c r="J430">
+        <v>0</v>
+      </c>
+      <c r="K430">
+        <v>0</v>
+      </c>
+      <c r="L430">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Slovakia: 2 reduced CIT rates
Introduction in 2025
</commit_message>
<xml_diff>
--- a/source_data/Tax Complexity Variable Notes.xlsx
+++ b/source_data/Tax Complexity Variable Notes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\international-tax-competitiveness-index\source_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BA6A4D4-7B47-4813-97C6-AAA3084278EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{819BA569-E9B9-49DF-81E8-FF42647E0EC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" xr2:uid="{799C6252-BD7E-43F6-A84E-AA4474677B14}"/>
   </bookViews>
@@ -152,7 +152,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2551" uniqueCount="403">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2551" uniqueCount="404">
   <si>
     <t>Australia</t>
   </si>
@@ -3415,6 +3415,9 @@
   </si>
   <si>
     <t>Two CIT brackets: 23.2% and 19%</t>
+  </si>
+  <si>
+    <t>2 reduced rates + QMDTT</t>
   </si>
 </sst>
 </file>
@@ -3882,10 +3885,10 @@
   <dimension ref="A1:L455"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="59" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E260" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E397" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F277" sqref="F277"/>
+      <selection pane="bottomRight" activeCell="F432" sqref="F432"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.899999999999999" x14ac:dyDescent="0.65"/>
@@ -20189,10 +20192,10 @@
         <v>2025</v>
       </c>
       <c r="E431" s="3" t="s">
-        <v>369</v>
+        <v>403</v>
       </c>
       <c r="F431" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G431" s="3" t="s">
         <v>126</v>

</xml_diff>